<commit_message>
Update MATERIAL WITH STANDARD.xlsx with newer version
</commit_message>
<xml_diff>
--- a/MATERIAL WITH STANDARD.xlsx
+++ b/MATERIAL WITH STANDARD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\EXPORT\01. EXPORT DEVELOPMENT LIST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Hriday\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF351F43-B934-4F07-837B-1CBBE690F7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4E8A27-92F9-4205-AD63-F7C436705E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5D10E886-6CCD-4869-9333-1F6CFD062509}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="83">
   <si>
     <t>CUSTOMER</t>
   </si>
@@ -280,6 +280,18 @@
   </si>
   <si>
     <t>CLASS R (OLD STANDARD )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REINFORCEMENT </t>
+  </si>
+  <si>
+    <t>KEVLAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOMEX 4 PLY </t>
+  </si>
+  <si>
+    <t>---</t>
   </si>
 </sst>
 </file>
@@ -716,10 +728,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,13 +740,13 @@
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="53.28515625" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="5" max="6" width="53.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>46</v>
       </c>
@@ -751,13 +763,16 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -773,10 +788,13 @@
       <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -792,10 +810,13 @@
       <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -811,10 +832,13 @@
       <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -830,10 +854,13 @@
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -849,10 +876,13 @@
       <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -868,10 +898,13 @@
       <c r="E7" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -887,10 +920,13 @@
       <c r="E8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -906,10 +942,13 @@
       <c r="E9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -925,10 +964,13 @@
       <c r="E10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -944,10 +986,13 @@
       <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -961,37 +1006,43 @@
       <c r="E12" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F12" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="5"/>
+      <c r="F13" s="1"/>
       <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="5"/>
+      <c r="F14" s="1"/>
       <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="5"/>
+      <c r="F15" s="1"/>
       <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>11</v>
       </c>
@@ -1007,10 +1058,13 @@
       <c r="E16" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="6"/>
+      <c r="F16" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>12</v>
       </c>
@@ -1026,10 +1080,13 @@
       <c r="E17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="5"/>
+      <c r="F17" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="G17" s="5"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>13</v>
       </c>
@@ -1045,10 +1102,13 @@
       <c r="E18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>14</v>
       </c>
@@ -1064,10 +1124,13 @@
       <c r="E19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="5"/>
+      <c r="F19" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>15</v>
       </c>
@@ -1083,10 +1146,11 @@
       <c r="E20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="3"/>
       <c r="G20" s="5"/>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>16</v>
       </c>
@@ -1102,10 +1166,13 @@
       <c r="E21" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="5"/>
+      <c r="F21" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>17</v>
       </c>
@@ -1121,10 +1188,13 @@
       <c r="E22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="5"/>
+      <c r="F22" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>18</v>
       </c>
@@ -1140,10 +1210,13 @@
       <c r="E23" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F23" s="5"/>
+      <c r="F23" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>19</v>
       </c>
@@ -1159,10 +1232,13 @@
       <c r="E24" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="5"/>
+      <c r="F24" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>20</v>
       </c>
@@ -1178,10 +1254,13 @@
       <c r="E25" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F25" s="5"/>
+      <c r="F25" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>21</v>
       </c>
@@ -1197,10 +1276,13 @@
       <c r="E26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="5"/>
+      <c r="F26" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>22</v>
       </c>
@@ -1216,10 +1298,11 @@
       <c r="E27" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F27" s="5"/>
+      <c r="F27" s="3"/>
       <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>23</v>
       </c>
@@ -1235,10 +1318,13 @@
       <c r="E28" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F28" s="5"/>
+      <c r="F28" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G28" s="5"/>
-    </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>24</v>
       </c>
@@ -1254,10 +1340,13 @@
       <c r="E29" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F29" s="5"/>
+      <c r="F29" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G29" s="5"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>25</v>
       </c>
@@ -1273,10 +1362,13 @@
       <c r="E30" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F30" s="5"/>
+      <c r="F30" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>26</v>
       </c>
@@ -1292,10 +1384,13 @@
       <c r="E31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F31" s="5"/>
+      <c r="F31" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>27</v>
       </c>
@@ -1311,10 +1406,13 @@
       <c r="E32" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F32" s="5"/>
+      <c r="F32" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>28</v>
       </c>
@@ -1330,10 +1428,13 @@
       <c r="E33" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F33" s="5"/>
+      <c r="F33" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G33" s="5"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>29</v>
       </c>
@@ -1349,10 +1450,13 @@
       <c r="E34" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F34" s="5"/>
+      <c r="F34" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G34" s="5"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>30</v>
       </c>
@@ -1368,10 +1472,13 @@
       <c r="E35" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F35" s="5"/>
+      <c r="F35" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G35" s="5"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>31</v>
       </c>
@@ -1387,10 +1494,13 @@
       <c r="E36" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F36" s="5"/>
+      <c r="F36" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G36" s="5"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
         <v>51</v>
@@ -1404,10 +1514,13 @@
       <c r="E37" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F37" s="5"/>
+      <c r="F37" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G37" s="5"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="5"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>32</v>
       </c>
@@ -1423,10 +1536,13 @@
       <c r="E38" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F38" s="5"/>
+      <c r="F38" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G38" s="5"/>
-    </row>
-    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>33</v>
       </c>
@@ -1442,10 +1558,13 @@
       <c r="E39" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F39" s="5"/>
+      <c r="F39" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G39" s="5"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
         <v>51</v>
@@ -1459,10 +1578,11 @@
       <c r="E40" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F40" s="5"/>
+      <c r="F40" s="3"/>
       <c r="G40" s="5"/>
-    </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>34</v>
       </c>
@@ -1478,8 +1598,11 @@
       <c r="E41" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F41" s="5"/>
+      <c r="F41" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update MATERIAL WITH STANDARD.xlsx with reinforcement data
</commit_message>
<xml_diff>
--- a/MATERIAL WITH STANDARD.xlsx
+++ b/MATERIAL WITH STANDARD.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Hriday\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EXP-24\Desktop\Feasibility 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4E8A27-92F9-4205-AD63-F7C436705E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94636953-73AC-48D1-9D66-848B48C25668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5D10E886-6CCD-4869-9333-1F6CFD062509}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{5D10E886-6CCD-4869-9333-1F6CFD062509}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Reinforcement" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="83">
   <si>
     <t>CUSTOMER</t>
   </si>
@@ -730,8 +731,8 @@
   </sheetPr>
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,4 +1609,569 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="61" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E0761A-59C1-4EB9-9111-0FB0DCE1A2FD}">
+  <dimension ref="A1:D41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>4496</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>4498</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>4542</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>